<commit_message>
Reading Index add dates
</commit_message>
<xml_diff>
--- a/Reading Index.xlsx
+++ b/Reading Index.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="99">
   <si>
     <t>Paper</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>8.19-8.20</t>
+  </si>
+  <si>
+    <t>8.17-8.18</t>
   </si>
 </sst>
 </file>
@@ -4315,10 +4318,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L995"/>
+  <dimension ref="A1:M995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4333,7 +4336,7 @@
     <col min="9" max="28" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>94</v>
       </c>
@@ -4370,8 +4373,11 @@
       <c r="L1">
         <v>8.16</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M1" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -4400,7 +4406,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -4428,7 +4434,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -4454,7 +4460,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -4489,7 +4495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -4513,7 +4519,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -4532,7 +4538,7 @@
       <c r="F7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -4559,7 +4565,7 @@
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -4590,7 +4596,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -4614,7 +4620,7 @@
         <v>8.17</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -4638,7 +4644,7 @@
         <v>8.18</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -4664,7 +4670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -4681,7 +4687,7 @@
       <c r="F13" s="3"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -4699,7 +4705,7 @@
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -4720,7 +4726,7 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>

</xml_diff>